<commit_message>
added tables and schemes
</commit_message>
<xml_diff>
--- a/instrumentace.xlsx
+++ b/instrumentace.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radim\Desktop\git\project_AUP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Skola - magistr\druhák\MPC-AUP\projekt\project_AUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED540781-8814-44E4-B24F-F36CEFBBCC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E23130-B464-447C-9C19-BB3E0DB3B0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3DF038C4-59DD-4D8C-89B0-4D36076B5952}"/>
+    <workbookView xWindow="6000" yWindow="468" windowWidth="18720" windowHeight="11628" xr2:uid="{3DF038C4-59DD-4D8C-89B0-4D36076B5952}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="138">
   <si>
     <t>Rozsah</t>
   </si>
@@ -391,6 +391,75 @@
   </si>
   <si>
     <t>závit M18</t>
+  </si>
+  <si>
+    <t>Typ modulu</t>
+  </si>
+  <si>
+    <t>MODULE1</t>
+  </si>
+  <si>
+    <t>MODULE2</t>
+  </si>
+  <si>
+    <t>MODULE3</t>
+  </si>
+  <si>
+    <t>KM1</t>
+  </si>
+  <si>
+    <t>FR1</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální vstupní/výstupní modul </t>
+  </si>
+  <si>
+    <t>Analogový výstupní modul</t>
+  </si>
+  <si>
+    <t>AQ 4xU/I HF</t>
+  </si>
+  <si>
+    <t>Analogový vstupní modul</t>
+  </si>
+  <si>
+    <t>AI 8xU/I/RTD BA</t>
+  </si>
+  <si>
+    <t>DI 16x24VDC DQ16x24VDC/0,5A</t>
+  </si>
+  <si>
+    <t>Popis</t>
+  </si>
+  <si>
+    <t>Poznámka</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>SIMATIC S7-1500</t>
+  </si>
+  <si>
+    <t>Zdroj</t>
+  </si>
+  <si>
+    <t>PS 25W 24 V DC</t>
+  </si>
+  <si>
+    <t>Stykač</t>
+  </si>
+  <si>
+    <t>Motorový spouštěč</t>
+  </si>
+  <si>
+    <t>Pojistka</t>
   </si>
 </sst>
 </file>
@@ -448,7 +517,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -583,12 +652,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -630,61 +740,79 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1002,48 +1130,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D7AA1C-20CF-4490-A041-11CADF853C8E}">
-  <dimension ref="A2:AF18"/>
+  <dimension ref="A2:AF29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="3.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="3.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.88671875" style="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="6" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="3.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="1"/>
+    <col min="14" max="14" width="3.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.109375" style="1" customWidth="1"/>
     <col min="16" max="16" width="13" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.44140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.88671875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" style="1" customWidth="1"/>
     <col min="22" max="22" width="7" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" style="1"/>
-    <col min="24" max="24" width="3.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="11.140625" style="1" customWidth="1"/>
-    <col min="26" max="27" width="12.140625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="12.5703125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="11.85546875" style="1" customWidth="1"/>
-    <col min="30" max="30" width="10.42578125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="13.28515625" style="1" customWidth="1"/>
-    <col min="32" max="32" width="6.85546875" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="1"/>
+    <col min="23" max="23" width="9.109375" style="1"/>
+    <col min="24" max="24" width="3.88671875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="11.109375" style="1" customWidth="1"/>
+    <col min="26" max="27" width="12.109375" style="1" customWidth="1"/>
+    <col min="28" max="28" width="12.5546875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.88671875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="10.44140625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="13.33203125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="6.88671875" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1054,8 +1182,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:32" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:32" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
         <v>8</v>
@@ -1138,7 +1266,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
         <v>1</v>
       </c>
@@ -1148,66 +1276,66 @@
       <c r="D5" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="29" t="s">
         <v>77</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="K5" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" s="21"/>
+      <c r="K5" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="29"/>
       <c r="N5" s="5">
         <v>1</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="P5" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="22" t="s">
+      <c r="Q5" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="R5" s="21" t="s">
+      <c r="R5" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="S5" s="21" t="s">
+      <c r="S5" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="21" t="s">
+      <c r="T5" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="V5" s="21"/>
+      <c r="U5" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="V5" s="29"/>
       <c r="X5" s="5">
         <v>1</v>
       </c>
       <c r="Y5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Z5" s="21" t="s">
+      <c r="Z5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="21" t="s">
+      <c r="AA5" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="AB5" s="21" t="s">
+      <c r="AB5" s="29" t="s">
         <v>28</v>
       </c>
       <c r="AC5" s="20" t="s">
@@ -1216,55 +1344,55 @@
       <c r="AD5" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="AE5" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF5" s="23"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE5" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF5" s="17"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="19"/>
       <c r="N6" s="7">
         <v>2</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
       <c r="U6" s="28"/>
-      <c r="V6" s="26"/>
+      <c r="V6" s="18"/>
       <c r="X6" s="7">
         <v>2</v>
       </c>
       <c r="Y6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="26"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="18"/>
       <c r="AE6" s="28"/>
-      <c r="AF6" s="26"/>
-    </row>
-    <row r="7" spans="1:32" ht="15" x14ac:dyDescent="0.2">
+      <c r="AF6" s="18"/>
+    </row>
+    <row r="7" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>3</v>
       </c>
@@ -1302,28 +1430,28 @@
       <c r="O7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="16"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="19"/>
       <c r="X7" s="7">
         <v>3</v>
       </c>
       <c r="Y7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="16"/>
-      <c r="AB7" s="16"/>
-      <c r="AC7" s="16"/>
-      <c r="AD7" s="16"/>
-      <c r="AE7" s="29"/>
-      <c r="AF7" s="16"/>
-    </row>
-    <row r="8" spans="1:32" ht="15" x14ac:dyDescent="0.2">
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="19"/>
+      <c r="AE7" s="26"/>
+      <c r="AF7" s="19"/>
+    </row>
+    <row r="8" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>4</v>
       </c>
@@ -1361,25 +1489,25 @@
       <c r="O8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="P8" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" s="31" t="s">
+      <c r="Q8" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="R8" s="25" t="s">
+      <c r="R8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="S8" s="25" t="s">
+      <c r="S8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="T8" s="19" t="s">
+      <c r="T8" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="U8" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="V8" s="19"/>
+      <c r="U8" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="V8" s="21"/>
       <c r="X8" s="7">
         <v>4</v>
       </c>
@@ -1406,7 +1534,7 @@
       </c>
       <c r="AF8" s="8"/>
     </row>
-    <row r="9" spans="1:32" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>5</v>
       </c>
@@ -1444,13 +1572,13 @@
       <c r="O9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
       <c r="U9" s="28"/>
-      <c r="V9" s="26"/>
+      <c r="V9" s="18"/>
       <c r="X9" s="7">
         <v>5</v>
       </c>
@@ -1477,7 +1605,7 @@
       </c>
       <c r="AF9" s="8"/>
     </row>
-    <row r="10" spans="1:32" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>6</v>
       </c>
@@ -1496,7 +1624,7 @@
       <c r="G10" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="H10" s="16" t="s">
         <v>109</v>
       </c>
       <c r="I10" s="8" t="s">
@@ -1515,40 +1643,40 @@
       <c r="O10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
       <c r="U10" s="28"/>
-      <c r="V10" s="26"/>
+      <c r="V10" s="18"/>
       <c r="X10" s="7">
         <v>6</v>
       </c>
       <c r="Y10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="Z10" s="19" t="s">
+      <c r="Z10" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="AA10" s="19" t="s">
+      <c r="AA10" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="AB10" s="19" t="s">
+      <c r="AB10" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AC10" s="25" t="s">
+      <c r="AC10" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="AD10" s="31" t="s">
+      <c r="AD10" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="AE10" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF10" s="19"/>
-    </row>
-    <row r="11" spans="1:32" ht="15" x14ac:dyDescent="0.2">
+      <c r="AE10" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF10" s="21"/>
+    </row>
+    <row r="11" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="7">
         <v>7</v>
@@ -1587,28 +1715,28 @@
       <c r="O11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="29"/>
-      <c r="V11" s="16"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="19"/>
       <c r="X11" s="7">
         <v>7</v>
       </c>
       <c r="Y11" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="Z11" s="16"/>
-      <c r="AA11" s="16"/>
-      <c r="AB11" s="16"/>
-      <c r="AC11" s="32"/>
-      <c r="AD11" s="16"/>
-      <c r="AE11" s="29"/>
-      <c r="AF11" s="16"/>
-    </row>
-    <row r="12" spans="1:32" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="23"/>
+      <c r="AD11" s="19"/>
+      <c r="AE11" s="26"/>
+      <c r="AF11" s="19"/>
+    </row>
+    <row r="12" spans="1:32" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>8</v>
       </c>
@@ -1666,70 +1794,280 @@
       </c>
       <c r="V12" s="8"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>9</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="K13" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="L13" s="19"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="K13" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="21"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>10</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="16"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="19"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="L16" s="11"/>
     </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L17" s="11"/>
     </row>
-    <row r="18" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="2"/>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="L18" s="11"/>
     </row>
+    <row r="19" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B20" s="7">
+        <v>2</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="2:12" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="7">
+        <v>3</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B22" s="7">
+        <v>4</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B23" s="7">
+        <v>5</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="39"/>
+      <c r="C25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B27" s="7">
+        <v>2</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="7">
+        <v>3</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="7">
+        <v>4</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="37"/>
+      <c r="E29" s="38"/>
+    </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="48">
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="Q5:Q7"/>
+    <mergeCell ref="P5:P7"/>
+    <mergeCell ref="R5:R7"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="S5:S7"/>
+    <mergeCell ref="T5:T7"/>
+    <mergeCell ref="U8:U11"/>
+    <mergeCell ref="V8:V11"/>
+    <mergeCell ref="V5:V7"/>
+    <mergeCell ref="U5:U7"/>
+    <mergeCell ref="P8:P11"/>
+    <mergeCell ref="Q8:Q11"/>
+    <mergeCell ref="R8:R11"/>
+    <mergeCell ref="S8:S11"/>
+    <mergeCell ref="T8:T11"/>
     <mergeCell ref="AF5:AF7"/>
     <mergeCell ref="AD5:AD7"/>
     <mergeCell ref="Z10:Z11"/>
@@ -1744,38 +2082,6 @@
     <mergeCell ref="AB5:AB7"/>
     <mergeCell ref="AC5:AC7"/>
     <mergeCell ref="Z5:Z7"/>
-    <mergeCell ref="P8:P11"/>
-    <mergeCell ref="Q8:Q11"/>
-    <mergeCell ref="R8:R11"/>
-    <mergeCell ref="S8:S11"/>
-    <mergeCell ref="T8:T11"/>
-    <mergeCell ref="S5:S7"/>
-    <mergeCell ref="T5:T7"/>
-    <mergeCell ref="U8:U11"/>
-    <mergeCell ref="V8:V11"/>
-    <mergeCell ref="V5:V7"/>
-    <mergeCell ref="U5:U7"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="Q5:Q7"/>
-    <mergeCell ref="P5:P7"/>
-    <mergeCell ref="R5:R7"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -1794,8 +2100,16 @@
     <hyperlink ref="K11" r:id="rId13" xr:uid="{202B5A24-7105-44E4-911C-07CADB855E11}"/>
     <hyperlink ref="K10" r:id="rId14" xr:uid="{38C66968-C7A8-4F98-80F9-7D676E68DD9A}"/>
     <hyperlink ref="K9" r:id="rId15" xr:uid="{408F019F-B266-4776-ACC9-2DE91432F16E}"/>
+    <hyperlink ref="F21" r:id="rId16" xr:uid="{B3F150E3-DB87-4868-8B37-BB3D13378DE2}"/>
+    <hyperlink ref="F19" r:id="rId17" xr:uid="{D7C911F9-EF9F-4D57-A048-912D5A33F552}"/>
+    <hyperlink ref="F20" r:id="rId18" xr:uid="{39999D14-59F4-4448-AA7A-675294D930F7}"/>
+    <hyperlink ref="F22" r:id="rId19" xr:uid="{6910AC38-9869-4AE5-9A22-E22ECE2403FB}"/>
+    <hyperlink ref="F23" r:id="rId20" xr:uid="{231AAE46-4AA4-4C92-9E45-80506D7D2CC2}"/>
+    <hyperlink ref="E26" r:id="rId21" xr:uid="{278F04A7-9F0B-4345-AAD9-70239AE02761}"/>
+    <hyperlink ref="E27" r:id="rId22" xr:uid="{36BF310F-5A7D-448C-B745-2C0DC47E584D}"/>
+    <hyperlink ref="E28:E29" r:id="rId23" display="URL" xr:uid="{0E4C73A2-8DF2-4377-AF66-E633928EA9B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>